<commit_message>
update with practice analysis
</commit_message>
<xml_diff>
--- a/Wolves_Filtered_100.xlsx
+++ b/Wolves_Filtered_100.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolyn/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolyn/Desktop/Practice_Data_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8243BD00-7D9E-3944-B7FB-7534CCB3803D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDF2A8B-5B5C-BE42-9292-B67A1DFCDB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{880A6FE7-E706-6844-BE22-28889B5D7842}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19300" xr2:uid="{880A6FE7-E706-6844-BE22-28889B5D7842}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1091,7 +1091,7 @@
   <dimension ref="A1:GA41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>